<commit_message>
add base library features
</commit_message>
<xml_diff>
--- a/Documentation/DEV Training 2025 - freshers-parth-sheladiya.xlsx
+++ b/Documentation/DEV Training 2025 - freshers-parth-sheladiya.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fb57ddd7d85ab252/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\parth-415\git-desk\RKIT_training\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_72089D55E0F912E4B708A5D8A6A30FE3087665EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DAA54E6E-45C6-442B-A224-AD41BF1DF329}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0A4046-A3F4-4498-97FD-EBAD20F71237}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name=" Basic GUI" sheetId="1" r:id="rId1"/>
@@ -21,17 +21,6 @@
     <sheet name="Deadline" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -2327,20 +2316,20 @@
       <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="6.77734375" customWidth="1"/>
+    <col min="1" max="1" width="6.75" customWidth="1"/>
     <col min="2" max="2" width="6" customWidth="1"/>
-    <col min="3" max="3" width="8.21875" customWidth="1"/>
-    <col min="4" max="4" width="37.88671875" customWidth="1"/>
-    <col min="5" max="5" width="53.33203125" customWidth="1"/>
-    <col min="6" max="7" width="9.21875" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="8.25" customWidth="1"/>
+    <col min="4" max="4" width="37.875" customWidth="1"/>
+    <col min="5" max="5" width="53.375" customWidth="1"/>
+    <col min="6" max="7" width="9.25" customWidth="1"/>
+    <col min="8" max="8" width="12.375" customWidth="1"/>
     <col min="9" max="9" width="13" customWidth="1"/>
-    <col min="10" max="10" width="21.44140625" customWidth="1"/>
-    <col min="11" max="11" width="25.109375" customWidth="1"/>
-    <col min="12" max="12" width="28.109375" customWidth="1"/>
-    <col min="13" max="26" width="8.6640625" customWidth="1"/>
+    <col min="10" max="10" width="21.5" customWidth="1"/>
+    <col min="11" max="11" width="25.125" customWidth="1"/>
+    <col min="12" max="12" width="28.125" customWidth="1"/>
+    <col min="13" max="26" width="8.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="18">
@@ -2383,7 +2372,7 @@
       <c r="Y1" s="3"/>
       <c r="Z1" s="3"/>
     </row>
-    <row r="2" spans="1:26" ht="18">
+    <row r="2" spans="1:26" ht="18.75">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -2421,7 +2410,7 @@
       <c r="Y2" s="11"/>
       <c r="Z2" s="11"/>
     </row>
-    <row r="3" spans="1:26" ht="15.6">
+    <row r="3" spans="1:26" ht="15.75">
       <c r="A3" s="12"/>
       <c r="B3" s="13">
         <v>1.1000000000000001</v>
@@ -2451,7 +2440,7 @@
       </c>
       <c r="L3" s="18"/>
     </row>
-    <row r="4" spans="1:26" ht="31.2">
+    <row r="4" spans="1:26" ht="31.5">
       <c r="A4" s="19"/>
       <c r="B4" s="20"/>
       <c r="C4" s="21" t="s">
@@ -2471,7 +2460,7 @@
       <c r="K4" s="18"/>
       <c r="L4" s="18"/>
     </row>
-    <row r="5" spans="1:26" ht="15.6">
+    <row r="5" spans="1:26" ht="15.75">
       <c r="A5" s="19"/>
       <c r="B5" s="20"/>
       <c r="C5" s="21" t="s">
@@ -2489,7 +2478,7 @@
       <c r="K5" s="18"/>
       <c r="L5" s="18"/>
     </row>
-    <row r="6" spans="1:26" ht="15.6">
+    <row r="6" spans="1:26" ht="15.75">
       <c r="A6" s="19"/>
       <c r="B6" s="20"/>
       <c r="C6" s="21" t="s">
@@ -2507,7 +2496,7 @@
       <c r="K6" s="18"/>
       <c r="L6" s="18"/>
     </row>
-    <row r="7" spans="1:26" ht="15.6">
+    <row r="7" spans="1:26" ht="15.75">
       <c r="A7" s="12"/>
       <c r="B7" s="24">
         <v>1.2</v>
@@ -2539,7 +2528,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="15.6">
+    <row r="8" spans="1:26" ht="15.75">
       <c r="A8" s="19"/>
       <c r="B8" s="20"/>
       <c r="C8" s="21" t="s">
@@ -2557,7 +2546,7 @@
       <c r="K8" s="18"/>
       <c r="L8" s="18"/>
     </row>
-    <row r="9" spans="1:26" ht="15.6">
+    <row r="9" spans="1:26" ht="15.75">
       <c r="A9" s="19"/>
       <c r="B9" s="20"/>
       <c r="C9" s="21" t="s">
@@ -2575,7 +2564,7 @@
       <c r="K9" s="18"/>
       <c r="L9" s="18"/>
     </row>
-    <row r="10" spans="1:26" ht="15.6">
+    <row r="10" spans="1:26" ht="15.75">
       <c r="A10" s="19"/>
       <c r="B10" s="20"/>
       <c r="C10" s="21" t="s">
@@ -2593,7 +2582,7 @@
       <c r="K10" s="18"/>
       <c r="L10" s="18"/>
     </row>
-    <row r="11" spans="1:26" ht="15.6">
+    <row r="11" spans="1:26" ht="15.75">
       <c r="A11" s="19"/>
       <c r="B11" s="20"/>
       <c r="C11" s="21" t="s">
@@ -2611,7 +2600,7 @@
       <c r="K11" s="18"/>
       <c r="L11" s="18"/>
     </row>
-    <row r="12" spans="1:26" ht="15.6">
+    <row r="12" spans="1:26" ht="15.75">
       <c r="A12" s="19"/>
       <c r="B12" s="20"/>
       <c r="C12" s="21" t="s">
@@ -2629,7 +2618,7 @@
       <c r="K12" s="18"/>
       <c r="L12" s="18"/>
     </row>
-    <row r="13" spans="1:26" ht="15.6">
+    <row r="13" spans="1:26" ht="15.75">
       <c r="A13" s="19"/>
       <c r="B13" s="20"/>
       <c r="C13" s="21" t="s">
@@ -2647,7 +2636,7 @@
       <c r="K13" s="18"/>
       <c r="L13" s="18"/>
     </row>
-    <row r="14" spans="1:26" ht="15.6">
+    <row r="14" spans="1:26" ht="15.75">
       <c r="A14" s="19"/>
       <c r="B14" s="20"/>
       <c r="C14" s="21" t="s">
@@ -2665,7 +2654,7 @@
       <c r="K14" s="18"/>
       <c r="L14" s="18"/>
     </row>
-    <row r="15" spans="1:26" ht="15.6">
+    <row r="15" spans="1:26" ht="15.75">
       <c r="A15" s="19"/>
       <c r="B15" s="20"/>
       <c r="C15" s="21" t="s">
@@ -2683,7 +2672,7 @@
       <c r="K15" s="18"/>
       <c r="L15" s="18"/>
     </row>
-    <row r="16" spans="1:26" ht="15.6">
+    <row r="16" spans="1:26" ht="15.75">
       <c r="A16" s="19"/>
       <c r="B16" s="20"/>
       <c r="C16" s="21" t="s">
@@ -2701,7 +2690,7 @@
       <c r="K16" s="18"/>
       <c r="L16" s="18"/>
     </row>
-    <row r="17" spans="1:12" ht="15.6">
+    <row r="17" spans="1:12" ht="15.75">
       <c r="A17" s="12"/>
       <c r="B17" s="24">
         <v>1.3</v>
@@ -2733,7 +2722,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="15.6">
+    <row r="18" spans="1:12" ht="15.75">
       <c r="A18" s="19"/>
       <c r="B18" s="20"/>
       <c r="C18" s="21" t="s">
@@ -2751,7 +2740,7 @@
       <c r="K18" s="18"/>
       <c r="L18" s="18"/>
     </row>
-    <row r="19" spans="1:12" ht="15.6">
+    <row r="19" spans="1:12" ht="15.75">
       <c r="A19" s="19"/>
       <c r="B19" s="20"/>
       <c r="C19" s="21" t="s">
@@ -2769,7 +2758,7 @@
       <c r="K19" s="18"/>
       <c r="L19" s="18"/>
     </row>
-    <row r="20" spans="1:12" ht="15.6">
+    <row r="20" spans="1:12" ht="15.75">
       <c r="A20" s="19"/>
       <c r="B20" s="20"/>
       <c r="C20" s="21" t="s">
@@ -11766,22 +11755,22 @@
       <selection activeCell="E76" sqref="E76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="25.88671875" customWidth="1"/>
-    <col min="3" max="3" width="65.6640625" customWidth="1"/>
-    <col min="4" max="4" width="7.77734375" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" customWidth="1"/>
-    <col min="6" max="6" width="14.44140625" customWidth="1"/>
-    <col min="7" max="7" width="8.44140625" customWidth="1"/>
-    <col min="8" max="8" width="17.88671875" customWidth="1"/>
-    <col min="9" max="9" width="20.77734375" customWidth="1"/>
-    <col min="10" max="10" width="30.6640625" customWidth="1"/>
-    <col min="11" max="26" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="25.875" customWidth="1"/>
+    <col min="3" max="3" width="65.625" customWidth="1"/>
+    <col min="4" max="4" width="7.75" customWidth="1"/>
+    <col min="5" max="5" width="8.375" customWidth="1"/>
+    <col min="6" max="6" width="14.5" customWidth="1"/>
+    <col min="7" max="7" width="8.5" customWidth="1"/>
+    <col min="8" max="8" width="17.875" customWidth="1"/>
+    <col min="9" max="9" width="20.75" customWidth="1"/>
+    <col min="10" max="10" width="30.625" customWidth="1"/>
+    <col min="11" max="26" width="8.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="14.4">
+    <row r="1" spans="1:26">
       <c r="A1" s="10" t="s">
         <v>178</v>
       </c>
@@ -11829,7 +11818,7 @@
       <c r="Y1" s="11"/>
       <c r="Z1" s="11"/>
     </row>
-    <row r="2" spans="1:26" ht="43.2">
+    <row r="2" spans="1:26" ht="43.5">
       <c r="A2" s="63" t="s">
         <v>183</v>
       </c>
@@ -11847,7 +11836,7 @@
       <c r="I2" s="18"/>
       <c r="J2" s="18"/>
     </row>
-    <row r="3" spans="1:26" ht="14.4">
+    <row r="3" spans="1:26">
       <c r="A3" s="63"/>
       <c r="B3" s="63"/>
       <c r="C3" s="18" t="s">
@@ -11871,7 +11860,7 @@
       <c r="I3" s="18"/>
       <c r="J3" s="18"/>
     </row>
-    <row r="4" spans="1:26" ht="14.4">
+    <row r="4" spans="1:26">
       <c r="A4" s="63" t="s">
         <v>187</v>
       </c>
@@ -11889,7 +11878,7 @@
       <c r="I4" s="18"/>
       <c r="J4" s="18"/>
     </row>
-    <row r="5" spans="1:26" ht="14.4">
+    <row r="5" spans="1:26">
       <c r="A5" s="63"/>
       <c r="B5" s="63"/>
       <c r="C5" s="18"/>
@@ -11901,7 +11890,7 @@
       <c r="I5" s="18"/>
       <c r="J5" s="18"/>
     </row>
-    <row r="6" spans="1:26" ht="14.4">
+    <row r="6" spans="1:26">
       <c r="A6" s="63" t="s">
         <v>190</v>
       </c>
@@ -11929,7 +11918,7 @@
       <c r="I6" s="18"/>
       <c r="J6" s="18"/>
     </row>
-    <row r="7" spans="1:26" ht="14.4">
+    <row r="7" spans="1:26">
       <c r="A7" s="63"/>
       <c r="B7" s="63"/>
       <c r="C7" s="18" t="s">
@@ -11951,7 +11940,7 @@
       <c r="I7" s="18"/>
       <c r="J7" s="18"/>
     </row>
-    <row r="8" spans="1:26" ht="14.4">
+    <row r="8" spans="1:26">
       <c r="A8" s="63"/>
       <c r="B8" s="63"/>
       <c r="C8" s="18" t="s">
@@ -11973,7 +11962,7 @@
       <c r="I8" s="18"/>
       <c r="J8" s="18"/>
     </row>
-    <row r="9" spans="1:26" ht="14.4">
+    <row r="9" spans="1:26">
       <c r="A9" s="63"/>
       <c r="B9" s="63"/>
       <c r="C9" s="18" t="s">
@@ -11995,7 +11984,7 @@
       <c r="I9" s="18"/>
       <c r="J9" s="18"/>
     </row>
-    <row r="10" spans="1:26" ht="14.4">
+    <row r="10" spans="1:26">
       <c r="A10" s="63"/>
       <c r="B10" s="63"/>
       <c r="C10" s="18" t="s">
@@ -12019,7 +12008,7 @@
       <c r="I10" s="18"/>
       <c r="J10" s="18"/>
     </row>
-    <row r="11" spans="1:26" ht="14.4">
+    <row r="11" spans="1:26">
       <c r="A11" s="63"/>
       <c r="B11" s="63"/>
       <c r="C11" s="18" t="s">
@@ -12041,7 +12030,7 @@
       <c r="I11" s="18"/>
       <c r="J11" s="18"/>
     </row>
-    <row r="12" spans="1:26" ht="14.4">
+    <row r="12" spans="1:26">
       <c r="A12" s="63"/>
       <c r="B12" s="63"/>
       <c r="C12" s="18" t="s">
@@ -12063,7 +12052,7 @@
       <c r="I12" s="18"/>
       <c r="J12" s="18"/>
     </row>
-    <row r="13" spans="1:26" ht="14.4">
+    <row r="13" spans="1:26">
       <c r="A13" s="63"/>
       <c r="B13" s="63"/>
       <c r="C13" s="18" t="s">
@@ -12085,7 +12074,7 @@
       <c r="I13" s="18"/>
       <c r="J13" s="18"/>
     </row>
-    <row r="14" spans="1:26" ht="14.4">
+    <row r="14" spans="1:26">
       <c r="A14" s="63"/>
       <c r="B14" s="63"/>
       <c r="C14" s="18" t="s">
@@ -12111,7 +12100,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="14.4">
+    <row r="15" spans="1:26">
       <c r="A15" s="63"/>
       <c r="B15" s="63"/>
       <c r="C15" s="18" t="s">
@@ -12133,7 +12122,7 @@
       <c r="I15" s="18"/>
       <c r="J15" s="18"/>
     </row>
-    <row r="16" spans="1:26" ht="14.4">
+    <row r="16" spans="1:26">
       <c r="A16" s="63"/>
       <c r="B16" s="63"/>
       <c r="C16" s="18" t="s">
@@ -12157,7 +12146,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="14.4">
+    <row r="17" spans="1:10">
       <c r="A17" s="63"/>
       <c r="B17" s="63"/>
       <c r="C17" s="18" t="s">
@@ -12179,7 +12168,7 @@
       <c r="I17" s="18"/>
       <c r="J17" s="66"/>
     </row>
-    <row r="18" spans="1:10" ht="14.4">
+    <row r="18" spans="1:10">
       <c r="A18" s="63"/>
       <c r="B18" s="63"/>
       <c r="C18" s="18" t="s">
@@ -12203,7 +12192,7 @@
       <c r="I18" s="18"/>
       <c r="J18" s="18"/>
     </row>
-    <row r="19" spans="1:10" ht="14.4">
+    <row r="19" spans="1:10">
       <c r="A19" s="63"/>
       <c r="B19" s="63"/>
       <c r="C19" s="18" t="s">
@@ -12225,7 +12214,7 @@
       <c r="I19" s="18"/>
       <c r="J19" s="18"/>
     </row>
-    <row r="20" spans="1:10" ht="14.4">
+    <row r="20" spans="1:10">
       <c r="A20" s="63"/>
       <c r="B20" s="63"/>
       <c r="C20" s="18" t="s">
@@ -20576,25 +20565,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="9.109375" customWidth="1"/>
-    <col min="2" max="2" width="25.21875" customWidth="1"/>
+    <col min="1" max="1" width="9.125" customWidth="1"/>
+    <col min="2" max="2" width="25.25" customWidth="1"/>
     <col min="3" max="3" width="43" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" customWidth="1"/>
-    <col min="6" max="6" width="6.6640625" customWidth="1"/>
-    <col min="7" max="7" width="8.44140625" customWidth="1"/>
-    <col min="8" max="8" width="17.21875" customWidth="1"/>
-    <col min="9" max="9" width="20.77734375" customWidth="1"/>
-    <col min="10" max="26" width="8.6640625" customWidth="1"/>
+    <col min="4" max="4" width="9.125" customWidth="1"/>
+    <col min="5" max="5" width="8.375" customWidth="1"/>
+    <col min="6" max="6" width="6.625" customWidth="1"/>
+    <col min="7" max="7" width="8.5" customWidth="1"/>
+    <col min="8" max="8" width="17.25" customWidth="1"/>
+    <col min="9" max="9" width="20.75" customWidth="1"/>
+    <col min="10" max="26" width="8.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="14.4">
+    <row r="1" spans="1:26">
       <c r="A1" s="10" t="s">
         <v>178</v>
       </c>
@@ -20642,7 +20631,7 @@
       <c r="Y1" s="11"/>
       <c r="Z1" s="11"/>
     </row>
-    <row r="2" spans="1:26" ht="14.4">
+    <row r="2" spans="1:26">
       <c r="A2" s="63" t="s">
         <v>183</v>
       </c>
@@ -20662,7 +20651,7 @@
       <c r="I2" s="18"/>
       <c r="J2" s="18"/>
     </row>
-    <row r="3" spans="1:26" ht="14.4">
+    <row r="3" spans="1:26">
       <c r="A3" s="63"/>
       <c r="B3" s="16"/>
       <c r="C3" s="18" t="s">
@@ -20676,7 +20665,7 @@
       <c r="I3" s="18"/>
       <c r="J3" s="18"/>
     </row>
-    <row r="4" spans="1:26" ht="14.4">
+    <row r="4" spans="1:26">
       <c r="A4" s="63"/>
       <c r="B4" s="16"/>
       <c r="C4" s="18" t="s">
@@ -20690,7 +20679,7 @@
       <c r="I4" s="18"/>
       <c r="J4" s="18"/>
     </row>
-    <row r="5" spans="1:26" ht="14.4">
+    <row r="5" spans="1:26">
       <c r="A5" s="63"/>
       <c r="B5" s="16"/>
       <c r="C5" s="18" t="s">
@@ -20704,7 +20693,7 @@
       <c r="I5" s="18"/>
       <c r="J5" s="18"/>
     </row>
-    <row r="6" spans="1:26" ht="14.4">
+    <row r="6" spans="1:26">
       <c r="A6" s="63"/>
       <c r="B6" s="16"/>
       <c r="C6" s="18" t="s">
@@ -20718,7 +20707,7 @@
       <c r="I6" s="18"/>
       <c r="J6" s="18"/>
     </row>
-    <row r="7" spans="1:26" ht="14.4">
+    <row r="7" spans="1:26">
       <c r="A7" s="63"/>
       <c r="B7" s="16"/>
       <c r="C7" s="18" t="s">
@@ -20732,7 +20721,7 @@
       <c r="I7" s="18"/>
       <c r="J7" s="18"/>
     </row>
-    <row r="8" spans="1:26" ht="14.4">
+    <row r="8" spans="1:26">
       <c r="A8" s="63"/>
       <c r="B8" s="16"/>
       <c r="C8" s="18" t="s">
@@ -20746,7 +20735,7 @@
       <c r="I8" s="18"/>
       <c r="J8" s="18"/>
     </row>
-    <row r="9" spans="1:26" ht="14.4">
+    <row r="9" spans="1:26">
       <c r="A9" s="63"/>
       <c r="B9" s="16"/>
       <c r="C9" s="18"/>
@@ -20758,7 +20747,7 @@
       <c r="I9" s="18"/>
       <c r="J9" s="18"/>
     </row>
-    <row r="10" spans="1:26" ht="14.4">
+    <row r="10" spans="1:26">
       <c r="A10" s="63" t="s">
         <v>187</v>
       </c>
@@ -20778,7 +20767,7 @@
       <c r="I10" s="18"/>
       <c r="J10" s="18"/>
     </row>
-    <row r="11" spans="1:26" ht="14.4">
+    <row r="11" spans="1:26">
       <c r="A11" s="63"/>
       <c r="B11" s="16"/>
       <c r="C11" s="18" t="s">
@@ -20794,7 +20783,7 @@
       <c r="I11" s="18"/>
       <c r="J11" s="18"/>
     </row>
-    <row r="12" spans="1:26" ht="14.4">
+    <row r="12" spans="1:26">
       <c r="A12" s="63"/>
       <c r="B12" s="16"/>
       <c r="C12" s="18" t="s">
@@ -20810,7 +20799,7 @@
       <c r="I12" s="18"/>
       <c r="J12" s="18"/>
     </row>
-    <row r="13" spans="1:26" ht="14.4">
+    <row r="13" spans="1:26">
       <c r="A13" s="63"/>
       <c r="B13" s="16"/>
       <c r="C13" s="18" t="s">
@@ -20826,7 +20815,7 @@
       <c r="I13" s="18"/>
       <c r="J13" s="18"/>
     </row>
-    <row r="14" spans="1:26" ht="14.4">
+    <row r="14" spans="1:26">
       <c r="A14" s="63"/>
       <c r="B14" s="16"/>
       <c r="C14" s="18" t="s">
@@ -20842,7 +20831,7 @@
       <c r="I14" s="18"/>
       <c r="J14" s="18"/>
     </row>
-    <row r="15" spans="1:26" ht="14.4">
+    <row r="15" spans="1:26">
       <c r="A15" s="63"/>
       <c r="B15" s="16"/>
       <c r="C15" s="18" t="s">
@@ -20858,7 +20847,7 @@
       <c r="I15" s="18"/>
       <c r="J15" s="18"/>
     </row>
-    <row r="16" spans="1:26" ht="14.4">
+    <row r="16" spans="1:26">
       <c r="A16" s="63"/>
       <c r="B16" s="16"/>
       <c r="C16" s="18" t="s">
@@ -20874,7 +20863,7 @@
       <c r="I16" s="18"/>
       <c r="J16" s="18"/>
     </row>
-    <row r="17" spans="1:10" ht="14.4">
+    <row r="17" spans="1:10">
       <c r="A17" s="63"/>
       <c r="B17" s="16"/>
       <c r="C17" s="18" t="s">
@@ -20890,7 +20879,7 @@
       <c r="I17" s="18"/>
       <c r="J17" s="18"/>
     </row>
-    <row r="18" spans="1:10" ht="14.4">
+    <row r="18" spans="1:10">
       <c r="A18" s="63"/>
       <c r="B18" s="16"/>
       <c r="C18" s="18" t="s">
@@ -20906,7 +20895,7 @@
       <c r="I18" s="18"/>
       <c r="J18" s="18"/>
     </row>
-    <row r="19" spans="1:10" ht="14.4">
+    <row r="19" spans="1:10">
       <c r="A19" s="63"/>
       <c r="B19" s="16"/>
       <c r="C19" s="18" t="s">
@@ -20922,7 +20911,7 @@
       <c r="I19" s="18"/>
       <c r="J19" s="18"/>
     </row>
-    <row r="20" spans="1:10" ht="14.4">
+    <row r="20" spans="1:10">
       <c r="A20" s="63"/>
       <c r="B20" s="16"/>
       <c r="C20" s="18" t="s">
@@ -28854,23 +28843,23 @@
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="9.109375" customWidth="1"/>
-    <col min="2" max="2" width="40.6640625" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" customWidth="1"/>
+    <col min="1" max="1" width="9.125" customWidth="1"/>
+    <col min="2" max="2" width="40.625" customWidth="1"/>
+    <col min="3" max="3" width="10.125" customWidth="1"/>
     <col min="4" max="4" width="32" customWidth="1"/>
     <col min="5" max="5" width="5" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" customWidth="1"/>
-    <col min="7" max="7" width="6.6640625" customWidth="1"/>
-    <col min="8" max="8" width="8.44140625" customWidth="1"/>
-    <col min="9" max="9" width="17.21875" customWidth="1"/>
-    <col min="10" max="10" width="20.77734375" customWidth="1"/>
-    <col min="11" max="11" width="8.88671875" customWidth="1"/>
-    <col min="12" max="26" width="8.6640625" customWidth="1"/>
+    <col min="6" max="6" width="8.375" customWidth="1"/>
+    <col min="7" max="7" width="6.625" customWidth="1"/>
+    <col min="8" max="8" width="8.5" customWidth="1"/>
+    <col min="9" max="9" width="17.25" customWidth="1"/>
+    <col min="10" max="10" width="20.75" customWidth="1"/>
+    <col min="11" max="11" width="8.875" customWidth="1"/>
+    <col min="12" max="26" width="8.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="14.4">
+    <row r="1" spans="1:26">
       <c r="A1" s="10" t="s">
         <v>178</v>
       </c>
@@ -28920,7 +28909,7 @@
       <c r="Y1" s="11"/>
       <c r="Z1" s="11"/>
     </row>
-    <row r="2" spans="1:26" ht="14.4">
+    <row r="2" spans="1:26">
       <c r="A2" s="76">
         <v>1</v>
       </c>
@@ -28943,7 +28932,7 @@
       <c r="J2" s="18"/>
       <c r="K2" s="18"/>
     </row>
-    <row r="3" spans="1:26" ht="14.4">
+    <row r="3" spans="1:26">
       <c r="A3" s="76"/>
       <c r="B3" s="68"/>
       <c r="C3" s="16">
@@ -28960,7 +28949,7 @@
       <c r="J3" s="18"/>
       <c r="K3" s="18"/>
     </row>
-    <row r="4" spans="1:26" ht="14.4">
+    <row r="4" spans="1:26">
       <c r="A4" s="76"/>
       <c r="B4" s="68"/>
       <c r="C4" s="16">
@@ -28977,7 +28966,7 @@
       <c r="J4" s="18"/>
       <c r="K4" s="18"/>
     </row>
-    <row r="5" spans="1:26" ht="14.4">
+    <row r="5" spans="1:26">
       <c r="A5" s="76"/>
       <c r="B5" s="68"/>
       <c r="C5" s="16">
@@ -28994,7 +28983,7 @@
       <c r="J5" s="18"/>
       <c r="K5" s="18"/>
     </row>
-    <row r="6" spans="1:26" ht="14.4">
+    <row r="6" spans="1:26">
       <c r="A6" s="16"/>
       <c r="B6" s="68"/>
       <c r="C6" s="16">
@@ -29011,7 +29000,7 @@
       <c r="J6" s="18"/>
       <c r="K6" s="18"/>
     </row>
-    <row r="7" spans="1:26" ht="14.4">
+    <row r="7" spans="1:26">
       <c r="A7" s="16"/>
       <c r="B7" s="68"/>
       <c r="C7" s="16">
@@ -29028,7 +29017,7 @@
       <c r="J7" s="18"/>
       <c r="K7" s="18"/>
     </row>
-    <row r="8" spans="1:26" ht="14.4">
+    <row r="8" spans="1:26">
       <c r="A8" s="16"/>
       <c r="B8" s="68"/>
       <c r="C8" s="16">
@@ -29045,7 +29034,7 @@
       <c r="J8" s="18"/>
       <c r="K8" s="18"/>
     </row>
-    <row r="9" spans="1:26" ht="14.4">
+    <row r="9" spans="1:26">
       <c r="A9" s="63"/>
       <c r="B9" s="68"/>
       <c r="C9" s="16">
@@ -29062,7 +29051,7 @@
       <c r="J9" s="18"/>
       <c r="K9" s="18"/>
     </row>
-    <row r="10" spans="1:26" ht="14.4">
+    <row r="10" spans="1:26">
       <c r="A10" s="63"/>
       <c r="B10" s="68"/>
       <c r="C10" s="16"/>
@@ -29075,7 +29064,7 @@
       <c r="J10" s="18"/>
       <c r="K10" s="18"/>
     </row>
-    <row r="11" spans="1:26" ht="14.4">
+    <row r="11" spans="1:26">
       <c r="A11" s="63">
         <v>2</v>
       </c>
@@ -29098,7 +29087,7 @@
       <c r="J11" s="18"/>
       <c r="K11" s="18"/>
     </row>
-    <row r="12" spans="1:26" ht="14.4">
+    <row r="12" spans="1:26">
       <c r="A12" s="63"/>
       <c r="B12" s="68"/>
       <c r="C12" s="16">
@@ -29117,7 +29106,7 @@
       <c r="J12" s="18"/>
       <c r="K12" s="18"/>
     </row>
-    <row r="13" spans="1:26" ht="14.4">
+    <row r="13" spans="1:26">
       <c r="A13" s="16"/>
       <c r="B13" s="68"/>
       <c r="C13" s="16">
@@ -29133,7 +29122,7 @@
       <c r="J13" s="18"/>
       <c r="K13" s="18"/>
     </row>
-    <row r="14" spans="1:26" ht="14.4">
+    <row r="14" spans="1:26">
       <c r="A14" s="16"/>
       <c r="B14" s="68"/>
       <c r="C14" s="16">
@@ -29152,7 +29141,7 @@
       <c r="J14" s="18"/>
       <c r="K14" s="18"/>
     </row>
-    <row r="15" spans="1:26" ht="14.4">
+    <row r="15" spans="1:26">
       <c r="A15" s="63"/>
       <c r="B15" s="68"/>
       <c r="C15" s="16">
@@ -29171,7 +29160,7 @@
       <c r="J15" s="18"/>
       <c r="K15" s="18"/>
     </row>
-    <row r="16" spans="1:26" ht="14.4">
+    <row r="16" spans="1:26">
       <c r="A16" s="63"/>
       <c r="B16" s="68"/>
       <c r="C16" s="16"/>
@@ -29184,7 +29173,7 @@
       <c r="J16" s="18"/>
       <c r="K16" s="18"/>
     </row>
-    <row r="17" spans="1:11" ht="14.4">
+    <row r="17" spans="1:11">
       <c r="A17" s="63">
         <v>3</v>
       </c>
@@ -29207,7 +29196,7 @@
       <c r="J17" s="18"/>
       <c r="K17" s="18"/>
     </row>
-    <row r="18" spans="1:11" ht="14.4">
+    <row r="18" spans="1:11">
       <c r="A18" s="63"/>
       <c r="B18" s="68"/>
       <c r="C18" s="16">
@@ -29224,7 +29213,7 @@
       <c r="J18" s="18"/>
       <c r="K18" s="18"/>
     </row>
-    <row r="19" spans="1:11" ht="14.4">
+    <row r="19" spans="1:11">
       <c r="A19" s="63"/>
       <c r="B19" s="68"/>
       <c r="C19" s="16">
@@ -29241,7 +29230,7 @@
       <c r="J19" s="18"/>
       <c r="K19" s="18"/>
     </row>
-    <row r="20" spans="1:11" ht="14.4">
+    <row r="20" spans="1:11">
       <c r="A20" s="63"/>
       <c r="B20" s="68"/>
       <c r="C20" s="16">
@@ -37207,19 +37196,19 @@
       <selection activeCell="D111" sqref="D111"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="9.109375" customWidth="1"/>
-    <col min="2" max="3" width="8.6640625" customWidth="1"/>
-    <col min="4" max="4" width="66.88671875" customWidth="1"/>
-    <col min="5" max="5" width="24.33203125" customWidth="1"/>
-    <col min="6" max="6" width="5.21875" customWidth="1"/>
-    <col min="7" max="7" width="8.33203125" customWidth="1"/>
-    <col min="8" max="8" width="6.6640625" customWidth="1"/>
-    <col min="9" max="9" width="8.44140625" customWidth="1"/>
-    <col min="10" max="10" width="17.88671875" customWidth="1"/>
-    <col min="11" max="11" width="20.77734375" customWidth="1"/>
-    <col min="12" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="9.125" customWidth="1"/>
+    <col min="2" max="3" width="8.625" customWidth="1"/>
+    <col min="4" max="4" width="66.875" customWidth="1"/>
+    <col min="5" max="5" width="24.375" customWidth="1"/>
+    <col min="6" max="6" width="5.25" customWidth="1"/>
+    <col min="7" max="7" width="8.375" customWidth="1"/>
+    <col min="8" max="8" width="6.625" customWidth="1"/>
+    <col min="9" max="9" width="8.5" customWidth="1"/>
+    <col min="10" max="10" width="17.875" customWidth="1"/>
+    <col min="11" max="11" width="20.75" customWidth="1"/>
+    <col min="12" max="26" width="8.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.75" customHeight="1">
@@ -37238,7 +37227,7 @@
       <c r="K1" s="101"/>
       <c r="L1" s="102"/>
     </row>
-    <row r="2" spans="1:12" ht="14.4">
+    <row r="2" spans="1:12">
       <c r="A2" s="111" t="s">
         <v>310</v>
       </c>
@@ -37268,7 +37257,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.6">
+    <row r="3" spans="1:12" ht="15.75">
       <c r="A3" s="44"/>
       <c r="B3" s="80"/>
       <c r="C3" s="81"/>
@@ -37284,7 +37273,7 @@
       <c r="K3" s="18"/>
       <c r="L3" s="18"/>
     </row>
-    <row r="4" spans="1:12" ht="15.6">
+    <row r="4" spans="1:12" ht="15.75">
       <c r="A4" s="24">
         <v>1</v>
       </c>
@@ -37304,7 +37293,7 @@
       <c r="K4" s="18"/>
       <c r="L4" s="18"/>
     </row>
-    <row r="5" spans="1:12" ht="15.6">
+    <row r="5" spans="1:12" ht="15.75">
       <c r="A5" s="45"/>
       <c r="B5" s="82">
         <v>1.1000000000000001</v>
@@ -37324,7 +37313,7 @@
       <c r="K5" s="18"/>
       <c r="L5" s="18"/>
     </row>
-    <row r="6" spans="1:12" ht="15.6">
+    <row r="6" spans="1:12" ht="15.75">
       <c r="A6" s="45"/>
       <c r="B6" s="82">
         <v>1.2</v>
@@ -37344,7 +37333,7 @@
       <c r="K6" s="18"/>
       <c r="L6" s="18"/>
     </row>
-    <row r="7" spans="1:12" ht="15.6">
+    <row r="7" spans="1:12" ht="15.75">
       <c r="A7" s="45"/>
       <c r="B7" s="82">
         <v>1.3</v>
@@ -37364,7 +37353,7 @@
       <c r="K7" s="18"/>
       <c r="L7" s="18"/>
     </row>
-    <row r="8" spans="1:12" ht="15.6">
+    <row r="8" spans="1:12" ht="15.75">
       <c r="A8" s="45"/>
       <c r="B8" s="82"/>
       <c r="C8" s="84" t="s">
@@ -37382,7 +37371,7 @@
       <c r="K8" s="18"/>
       <c r="L8" s="18"/>
     </row>
-    <row r="9" spans="1:12" ht="15.6">
+    <row r="9" spans="1:12" ht="15.75">
       <c r="A9" s="45"/>
       <c r="B9" s="82"/>
       <c r="C9" s="84" t="s">
@@ -37400,7 +37389,7 @@
       <c r="K9" s="18"/>
       <c r="L9" s="18"/>
     </row>
-    <row r="10" spans="1:12" ht="15.6">
+    <row r="10" spans="1:12" ht="15.75">
       <c r="A10" s="45"/>
       <c r="B10" s="82"/>
       <c r="C10" s="84" t="s">
@@ -37418,7 +37407,7 @@
       <c r="K10" s="18"/>
       <c r="L10" s="18"/>
     </row>
-    <row r="11" spans="1:12" ht="15.6">
+    <row r="11" spans="1:12" ht="15.75">
       <c r="A11" s="45"/>
       <c r="B11" s="82"/>
       <c r="C11" s="84" t="s">
@@ -37436,7 +37425,7 @@
       <c r="K11" s="18"/>
       <c r="L11" s="18"/>
     </row>
-    <row r="12" spans="1:12" ht="15.6">
+    <row r="12" spans="1:12" ht="15.75">
       <c r="A12" s="45"/>
       <c r="B12" s="82"/>
       <c r="C12" s="84" t="s">
@@ -37454,7 +37443,7 @@
       <c r="K12" s="18"/>
       <c r="L12" s="18"/>
     </row>
-    <row r="13" spans="1:12" ht="15.6">
+    <row r="13" spans="1:12" ht="15.75">
       <c r="A13" s="45"/>
       <c r="B13" s="82"/>
       <c r="C13" s="84" t="s">
@@ -37472,7 +37461,7 @@
       <c r="K13" s="18"/>
       <c r="L13" s="18"/>
     </row>
-    <row r="14" spans="1:12" ht="15.6">
+    <row r="14" spans="1:12" ht="15.75">
       <c r="A14" s="45"/>
       <c r="B14" s="82"/>
       <c r="C14" s="84"/>
@@ -37486,7 +37475,7 @@
       <c r="K14" s="18"/>
       <c r="L14" s="18"/>
     </row>
-    <row r="15" spans="1:12" ht="15.6">
+    <row r="15" spans="1:12" ht="15.75">
       <c r="A15" s="24">
         <v>2</v>
       </c>
@@ -37508,7 +37497,7 @@
       <c r="K15" s="18"/>
       <c r="L15" s="18"/>
     </row>
-    <row r="16" spans="1:12" ht="15.6">
+    <row r="16" spans="1:12" ht="15.75">
       <c r="A16" s="45"/>
       <c r="B16" s="82">
         <v>2.1</v>
@@ -37528,7 +37517,7 @@
       <c r="K16" s="18"/>
       <c r="L16" s="18"/>
     </row>
-    <row r="17" spans="1:12" ht="15.6">
+    <row r="17" spans="1:12" ht="15.75">
       <c r="A17" s="45"/>
       <c r="B17" s="82">
         <v>2.2000000000000002</v>
@@ -37548,7 +37537,7 @@
       <c r="K17" s="18"/>
       <c r="L17" s="18"/>
     </row>
-    <row r="18" spans="1:12" ht="15.6">
+    <row r="18" spans="1:12" ht="15.75">
       <c r="A18" s="45"/>
       <c r="B18" s="82">
         <v>2.2999999999999998</v>
@@ -37568,7 +37557,7 @@
       <c r="K18" s="18"/>
       <c r="L18" s="18"/>
     </row>
-    <row r="19" spans="1:12" ht="15.6">
+    <row r="19" spans="1:12" ht="15.75">
       <c r="A19" s="45"/>
       <c r="B19" s="82">
         <v>2.4</v>
@@ -37588,7 +37577,7 @@
       <c r="K19" s="18"/>
       <c r="L19" s="18"/>
     </row>
-    <row r="20" spans="1:12" ht="15.6">
+    <row r="20" spans="1:12" ht="15.75">
       <c r="A20" s="45"/>
       <c r="B20" s="82">
         <v>2.5</v>
@@ -45573,15 +45562,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="14.21875" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.25" customWidth="1"/>
+    <col min="2" max="2" width="11.875" customWidth="1"/>
+    <col min="3" max="3" width="16.5" customWidth="1"/>
+    <col min="4" max="26" width="8.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14.4">
+    <row r="1" spans="1:3">
       <c r="A1" s="94" t="s">
         <v>446</v>
       </c>
@@ -45592,7 +45581,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14.4">
+    <row r="2" spans="1:3" ht="14.25">
       <c r="A2" s="97" t="s">
         <v>449</v>
       </c>

</xml_diff>